<commit_message>
Drop usage of FlaggedPatient
</commit_message>
<xml_diff>
--- a/sepsis/rules/sepsis_rules_table.drl.xlsx
+++ b/sepsis/rules/sepsis_rules_table.drl.xlsx
@@ -31,7 +31,7 @@
     <t xml:space="preserve">Import</t>
   </si>
   <si>
-    <t xml:space="preserve">org.openmrs.Patient,org.openmrs.module.drools.patientflags.FlaggedPatient,org.openmrs.module.drools.calculation.Operator, static org.openmrs.module.drools.utils.DroolsDateUtils.daysAgo</t>
+    <t xml:space="preserve">org.openmrs.Patient,org.openmrs.module.patientflags.PatientFlag,org.openmrs.module.drools.calculation.Operator, static org.openmrs.module.drools.utils.DroolsDateUtils.daysAgo</t>
   </si>
   <si>
     <t xml:space="preserve">Variables</t>
@@ -88,13 +88,13 @@
     <t xml:space="preserve">service.checkObs($patient, "CIEL:5085", Operator.GTE, daysAgo(1)).matches(Operator.LT, $param)</t>
   </si>
   <si>
-    <t xml:space="preserve">not FlaggedPatient(patientId == $patient.getId())</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$flag: FlaggedPatient(patientId == $patient.getId(), message == $param)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">insert(new FlaggedPatient($patient.getId(), $param));</t>
+    <t xml:space="preserve">not PatientFlag(patient == $patient)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$flag: PatientFlag(patient == $patient, message == $param)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">insert(new PatientFlag($patient, null, $param));</t>
   </si>
   <si>
     <t xml:space="preserve">modify($flag){ setMessage($param) }</t>
@@ -503,7 +503,7 @@
   <dimension ref="A1:K1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.515625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -517,7 +517,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="34.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="34.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="3" width="23.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="3" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>